<commit_message>
Fixed Tomas process evaulation
</commit_message>
<xml_diff>
--- a/example/B.xlsx
+++ b/example/B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\aspice-reporting\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8528930C-9281-4F57-BBDF-7D6C4C23FFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B21C75-9465-46AE-8CC1-D94B797BD496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6945" yWindow="3120" windowWidth="14025" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10350" yWindow="1665" windowWidth="14025" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="55">
   <si>
     <t>ACQ.4</t>
   </si>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F161" sqref="F161:G161"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,10 +2347,10 @@
         <v>48</v>
       </c>
       <c r="F79" t="s">
-        <v>32</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="G79" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -2370,10 +2370,10 @@
         <v>48</v>
       </c>
       <c r="F80" t="s">
-        <v>32</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="G80" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>